<commit_message>
Inclusão dos mapas de ocorrencia dos invertebrados
</commit_message>
<xml_diff>
--- a/invertebrados/ocorrencias/Validado_Bivalvia_consolidado_05abr23.xlsx
+++ b/invertebrados/ocorrencias/Validado_Bivalvia_consolidado_05abr23.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Taise\bluePrintAraguaia\Dados\Invertebrados\bivalvia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Taise\mapasAraguaia\invertebrados\ocorrencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12D24C8-E97B-4944-AFE8-2F45C78C1B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE428431-4525-4823-819E-F8298B7A6794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$AH$1:$BE$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$AH$1:$BF$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
     <author>tc={7A7CC9AA-CD6E-48B2-8C15-A9737EEBBE68}</author>
   </authors>
   <commentList>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{285806BF-BE51-4B1E-A007-B1C5ABCA9155}">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{285806BF-BE51-4B1E-A007-B1C5ABCA9155}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -48,7 +48,7 @@
 Que nível de endemismo?</t>
       </text>
     </comment>
-    <comment ref="BB1" authorId="1" shapeId="0" xr:uid="{7A7CC9AA-CD6E-48B2-8C15-A9737EEBBE68}">
+    <comment ref="BC1" authorId="1" shapeId="0" xr:uid="{7A7CC9AA-CD6E-48B2-8C15-A9737EEBBE68}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="619">
   <si>
     <t>id</t>
   </si>
@@ -1912,6 +1912,12 @@
   </si>
   <si>
     <t>Deletar</t>
+  </si>
+  <si>
+    <t>origem</t>
+  </si>
+  <si>
+    <t>nativo</t>
   </si>
 </sst>
 </file>
@@ -2310,11 +2316,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="AW1" dT="2023-04-03T20:46:51.96" personId="{82B2C2A1-1D06-4A15-A051-F1E49BBD9DD0}" id="{285806BF-BE51-4B1E-A007-B1C5ABCA9155}">
+  <threadedComment ref="AX1" dT="2023-04-03T20:46:51.96" personId="{82B2C2A1-1D06-4A15-A051-F1E49BBD9DD0}" id="{285806BF-BE51-4B1E-A007-B1C5ABCA9155}">
     <text>Confirmar com Milena.
 Que nível de endemismo?</text>
   </threadedComment>
-  <threadedComment ref="BB1" dT="2023-04-03T20:39:41.66" personId="{82B2C2A1-1D06-4A15-A051-F1E49BBD9DD0}" id="{7A7CC9AA-CD6E-48B2-8C15-A9737EEBBE68}">
+  <threadedComment ref="BC1" dT="2023-04-03T20:39:41.66" personId="{82B2C2A1-1D06-4A15-A051-F1E49BBD9DD0}" id="{7A7CC9AA-CD6E-48B2-8C15-A9737EEBBE68}">
     <text>ALÓCTONE / AUTÓCTONE (EXÓTICA?)</text>
   </threadedComment>
 </ThreadedComments>
@@ -2322,12 +2328,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE103"/>
+  <dimension ref="A1:BF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE1" sqref="AE1"/>
-      <selection pane="bottomLeft" activeCell="AJ14" sqref="AH2:AJ14"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,13 +2345,13 @@
     <col min="28" max="28" width="51" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="24" customWidth="1"/>
     <col min="35" max="35" width="48.28515625" customWidth="1"/>
-    <col min="36" max="36" width="29.140625" customWidth="1"/>
-    <col min="55" max="55" width="15.85546875" customWidth="1"/>
-    <col min="56" max="56" width="17.85546875" customWidth="1"/>
-    <col min="57" max="57" width="19.140625" customWidth="1"/>
+    <col min="36" max="37" width="29.140625" customWidth="1"/>
+    <col min="56" max="56" width="15.85546875" customWidth="1"/>
+    <col min="57" max="57" width="17.85546875" customWidth="1"/>
+    <col min="58" max="58" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2449,73 +2455,76 @@
         <v>569</v>
       </c>
       <c r="AJ1" t="s">
+        <v>617</v>
+      </c>
+      <c r="AK1" t="s">
         <v>570</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2594,11 +2603,14 @@
       <c r="AJ2" t="s">
         <v>588</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="AK2" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC2" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>304</v>
       </c>
@@ -2689,11 +2701,14 @@
       <c r="AJ3" t="s">
         <v>588</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="AK3" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC3" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>333</v>
       </c>
@@ -2784,11 +2799,14 @@
       <c r="AJ4" t="s">
         <v>588</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="AK4" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC4" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>370</v>
       </c>
@@ -2855,11 +2873,14 @@
       <c r="AJ5" t="s">
         <v>588</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="AK5" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC5" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>376</v>
       </c>
@@ -2926,11 +2947,14 @@
       <c r="AJ6" t="s">
         <v>588</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="AK6" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC6" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>384</v>
       </c>
@@ -2997,11 +3021,14 @@
       <c r="AJ7" t="s">
         <v>588</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="AK7" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC7" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>414</v>
       </c>
@@ -3059,11 +3086,14 @@
       <c r="AJ8" t="s">
         <v>588</v>
       </c>
-      <c r="BB8" t="s">
+      <c r="AK8" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC8" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>435</v>
       </c>
@@ -3121,11 +3151,14 @@
       <c r="AJ9" t="s">
         <v>588</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="AK9" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC9" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>468</v>
       </c>
@@ -3192,11 +3225,14 @@
       <c r="AJ10" t="s">
         <v>588</v>
       </c>
-      <c r="BB10" t="s">
+      <c r="AK10" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC10" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>473</v>
       </c>
@@ -3263,11 +3299,14 @@
       <c r="AJ11" t="s">
         <v>588</v>
       </c>
-      <c r="BB11" t="s">
+      <c r="AK11" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC11" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>478</v>
       </c>
@@ -3334,11 +3373,14 @@
       <c r="AJ12" t="s">
         <v>588</v>
       </c>
-      <c r="BB12" t="s">
+      <c r="AK12" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC12" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>482</v>
       </c>
@@ -3405,11 +3447,14 @@
       <c r="AJ13" t="s">
         <v>588</v>
       </c>
-      <c r="BB13" t="s">
+      <c r="AK13" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC13" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>486</v>
       </c>
@@ -3476,11 +3521,14 @@
       <c r="AJ14" t="s">
         <v>588</v>
       </c>
-      <c r="BB14" t="s">
+      <c r="AK14" t="s">
+        <v>588</v>
+      </c>
+      <c r="BC14" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -3565,8 +3613,11 @@
       <c r="AF15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ15" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -3651,8 +3702,11 @@
       <c r="AF16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ16" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -3738,10 +3792,13 @@
         <v>51</v>
       </c>
       <c r="AJ17" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK17" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3824,10 +3881,13 @@
         <v>125</v>
       </c>
       <c r="AJ18" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK18" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -3910,10 +3970,13 @@
         <v>167</v>
       </c>
       <c r="AJ19" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK19" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>168</v>
       </c>
@@ -3996,10 +4059,13 @@
         <v>175</v>
       </c>
       <c r="AJ20" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK20" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -4082,10 +4148,13 @@
         <v>182</v>
       </c>
       <c r="AJ21" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK21" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -4168,10 +4237,13 @@
         <v>189</v>
       </c>
       <c r="AJ22" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK22" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="23" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>190</v>
       </c>
@@ -4253,17 +4325,20 @@
       <c r="AF23" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="AJ23" s="5" t="s">
+      <c r="AJ23" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK23" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="BD23" s="5" t="s">
+      <c r="BE23" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="BE23" s="5" t="s">
+      <c r="BF23" s="5" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -4348,8 +4423,11 @@
       <c r="AF24" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ24" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>226</v>
       </c>
@@ -4435,10 +4513,13 @@
         <v>231</v>
       </c>
       <c r="AJ25" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK25" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>232</v>
       </c>
@@ -4523,8 +4604,11 @@
       <c r="AF26" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ26" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>252</v>
       </c>
@@ -4609,8 +4693,11 @@
       <c r="AF27" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ27" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>264</v>
       </c>
@@ -4695,8 +4782,11 @@
       <c r="AF28" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ28" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>308</v>
       </c>
@@ -4781,8 +4871,11 @@
       <c r="AF29" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ29" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>314</v>
       </c>
@@ -4867,8 +4960,11 @@
       <c r="AF30" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ30" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>316</v>
       </c>
@@ -4953,8 +5049,11 @@
       <c r="AF31" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ31" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>318</v>
       </c>
@@ -5039,8 +5138,11 @@
       <c r="AF32" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ32" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>327</v>
       </c>
@@ -5125,8 +5227,11 @@
       <c r="AF33" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ33" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>335</v>
       </c>
@@ -5205,8 +5310,11 @@
       <c r="AF34" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ34" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>342</v>
       </c>
@@ -5288,8 +5396,11 @@
       <c r="AF35" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ35" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>349</v>
       </c>
@@ -5371,8 +5482,11 @@
       <c r="AF36" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ36" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>357</v>
       </c>
@@ -5455,10 +5569,13 @@
         <v>348</v>
       </c>
       <c r="AJ37" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK37" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>359</v>
       </c>
@@ -5540,8 +5657,11 @@
       <c r="AF38" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ38" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>390</v>
       </c>
@@ -5599,8 +5719,11 @@
       <c r="AF39" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ39" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>396</v>
       </c>
@@ -5658,8 +5781,11 @@
       <c r="AF40" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ40" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>404</v>
       </c>
@@ -5712,10 +5838,13 @@
         <v>408</v>
       </c>
       <c r="AJ41" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK41" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>409</v>
       </c>
@@ -5767,8 +5896,11 @@
       <c r="AF42" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ42" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>420</v>
       </c>
@@ -5820,8 +5952,11 @@
       <c r="AF43" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ43" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>425</v>
       </c>
@@ -5873,8 +6008,11 @@
       <c r="AF44" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ44" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>430</v>
       </c>
@@ -5926,8 +6064,11 @@
       <c r="AF45" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ45" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>442</v>
       </c>
@@ -5979,8 +6120,11 @@
       <c r="AF46" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ46" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>444</v>
       </c>
@@ -6032,8 +6176,11 @@
       <c r="AF47" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ47" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>451</v>
       </c>
@@ -6085,8 +6232,11 @@
       <c r="AF48" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ48" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>456</v>
       </c>
@@ -6138,8 +6288,11 @@
       <c r="AF49" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ49" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>461</v>
       </c>
@@ -6191,8 +6344,11 @@
       <c r="AF50" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ50" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>491</v>
       </c>
@@ -6247,8 +6403,11 @@
       <c r="AF51" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ51" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>500</v>
       </c>
@@ -6303,8 +6462,11 @@
       <c r="AF52" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ52" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>506</v>
       </c>
@@ -6359,8 +6521,11 @@
       <c r="AF53" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ53" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>509</v>
       </c>
@@ -6415,8 +6580,11 @@
       <c r="AF54" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ54" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>511</v>
       </c>
@@ -6471,8 +6639,11 @@
       <c r="AF55" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ55" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>522</v>
       </c>
@@ -6527,8 +6698,11 @@
       <c r="AF56" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ56" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>523</v>
       </c>
@@ -6583,8 +6757,11 @@
       <c r="AF57" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ57" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>527</v>
       </c>
@@ -6639,8 +6816,11 @@
       <c r="AF58" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ58" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>532</v>
       </c>
@@ -6695,8 +6875,11 @@
       <c r="AF59" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ59" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>542</v>
       </c>
@@ -6749,10 +6932,13 @@
         <v>539</v>
       </c>
       <c r="AJ60" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK60" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>543</v>
       </c>
@@ -6804,8 +6990,11 @@
       <c r="AF61" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ61" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>545</v>
       </c>
@@ -6857,8 +7046,11 @@
       <c r="AF62" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ62" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>546</v>
       </c>
@@ -6910,8 +7102,11 @@
       <c r="AF63" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AJ63" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>547</v>
       </c>
@@ -6963,8 +7158,11 @@
       <c r="AF64" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="65" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ64" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>549</v>
       </c>
@@ -7017,10 +7215,13 @@
         <v>51</v>
       </c>
       <c r="AJ65" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>567</v>
       </c>
@@ -7073,10 +7274,13 @@
         <v>51</v>
       </c>
       <c r="AJ66" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK66" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="67" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>126</v>
       </c>
@@ -7155,8 +7359,11 @@
       <c r="AI67" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ67" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>551</v>
       </c>
@@ -7214,8 +7421,11 @@
       <c r="AI68" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="69" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ68" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>554</v>
       </c>
@@ -7274,10 +7484,13 @@
         <v>613</v>
       </c>
       <c r="AJ69" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK69" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>556</v>
       </c>
@@ -7327,10 +7540,13 @@
         <v>614</v>
       </c>
       <c r="AJ70" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK70" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="71" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -7406,14 +7622,17 @@
       <c r="AF71" t="s">
         <v>51</v>
       </c>
-      <c r="BD71" t="s">
+      <c r="AJ71" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE71" t="s">
         <v>595</v>
       </c>
-      <c r="BE71" t="s">
+      <c r="BF71" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="72" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -7504,8 +7723,11 @@
       <c r="AI72" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ72" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>151</v>
       </c>
@@ -7584,14 +7806,17 @@
       <c r="AF73" t="s">
         <v>158</v>
       </c>
-      <c r="BD73" t="s">
+      <c r="AJ73" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE73" t="s">
         <v>595</v>
       </c>
-      <c r="BE73" t="s">
+      <c r="BF73" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="74" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>212</v>
       </c>
@@ -7676,14 +7901,17 @@
       <c r="AF74" t="s">
         <v>219</v>
       </c>
-      <c r="BD74" t="s">
+      <c r="AJ74" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE74" t="s">
         <v>595</v>
       </c>
-      <c r="BE74" t="s">
+      <c r="BF74" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="75" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>220</v>
       </c>
@@ -7768,14 +7996,17 @@
       <c r="AF75" t="s">
         <v>225</v>
       </c>
-      <c r="BD75" t="s">
+      <c r="AJ75" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE75" t="s">
         <v>595</v>
       </c>
-      <c r="BE75" t="s">
+      <c r="BF75" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="76" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>240</v>
       </c>
@@ -7860,14 +8091,17 @@
       <c r="AF76" t="s">
         <v>239</v>
       </c>
-      <c r="BD76" t="s">
+      <c r="AJ76" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE76" t="s">
         <v>595</v>
       </c>
-      <c r="BE76" t="s">
+      <c r="BF76" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="77" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>242</v>
       </c>
@@ -7953,10 +8187,13 @@
         <v>251</v>
       </c>
       <c r="AJ77" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK77" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="78" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>275</v>
       </c>
@@ -8041,14 +8278,17 @@
       <c r="AF78" t="s">
         <v>284</v>
       </c>
-      <c r="BD78" t="s">
+      <c r="AJ78" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE78" t="s">
         <v>597</v>
       </c>
-      <c r="BE78" t="s">
+      <c r="BF78" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="79" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>285</v>
       </c>
@@ -8133,14 +8373,17 @@
       <c r="AF79" t="s">
         <v>290</v>
       </c>
-      <c r="BD79" t="s">
+      <c r="AJ79" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE79" t="s">
         <v>598</v>
       </c>
-      <c r="BE79" t="s">
+      <c r="BF79" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="80" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>291</v>
       </c>
@@ -8225,14 +8468,17 @@
       <c r="AF80" t="s">
         <v>296</v>
       </c>
-      <c r="BD80" t="s">
+      <c r="AJ80" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE80" t="s">
         <v>598</v>
       </c>
-      <c r="BE80" t="s">
+      <c r="BF80" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="81" spans="1:57" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:58" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>297</v>
       </c>
@@ -8317,17 +8563,20 @@
       <c r="AF81" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="AJ81" s="6" t="s">
+      <c r="AJ81" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK81" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="BD81" s="6" t="s">
+      <c r="BE81" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="BE81" s="6" t="s">
+      <c r="BF81" s="6" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="82" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>321</v>
       </c>
@@ -8412,14 +8661,17 @@
       <c r="AF82" t="s">
         <v>326</v>
       </c>
-      <c r="BD82" t="s">
+      <c r="AJ82" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE82" t="s">
         <v>595</v>
       </c>
-      <c r="BE82" t="s">
+      <c r="BF82" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="83" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>352</v>
       </c>
@@ -8501,14 +8753,17 @@
       <c r="AF83" t="s">
         <v>348</v>
       </c>
-      <c r="BD83" t="s">
+      <c r="AJ83" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE83" t="s">
         <v>595</v>
       </c>
-      <c r="BE83" t="s">
+      <c r="BF83" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="84" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>361</v>
       </c>
@@ -8590,14 +8845,17 @@
       <c r="AF84" t="s">
         <v>348</v>
       </c>
-      <c r="BD84" t="s">
+      <c r="AJ84" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE84" t="s">
         <v>595</v>
       </c>
-      <c r="BE84" t="s">
+      <c r="BF84" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="85" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>363</v>
       </c>
@@ -8679,8 +8937,11 @@
       <c r="AF85" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="86" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ85" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>398</v>
       </c>
@@ -8738,14 +8999,17 @@
       <c r="AF86" t="s">
         <v>395</v>
       </c>
-      <c r="BD86" t="s">
+      <c r="AJ86" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE86" t="s">
         <v>595</v>
       </c>
-      <c r="BE86" t="s">
+      <c r="BF86" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="87" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>401</v>
       </c>
@@ -8803,8 +9067,11 @@
       <c r="AF87" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="88" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ87" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>440</v>
       </c>
@@ -8856,14 +9123,17 @@
       <c r="AF88" t="s">
         <v>439</v>
       </c>
-      <c r="BD88" t="s">
+      <c r="AJ88" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE88" t="s">
         <v>595</v>
       </c>
-      <c r="BE88" t="s">
+      <c r="BF88" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="89" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>449</v>
       </c>
@@ -8915,14 +9185,17 @@
       <c r="AF89" t="s">
         <v>408</v>
       </c>
-      <c r="BD89" t="s">
+      <c r="AJ89" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE89" t="s">
         <v>595</v>
       </c>
-      <c r="BE89" t="s">
+      <c r="BF89" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="90" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>463</v>
       </c>
@@ -8974,14 +9247,17 @@
       <c r="AF90" t="s">
         <v>467</v>
       </c>
-      <c r="BD90" t="s">
+      <c r="AJ90" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE90" t="s">
         <v>598</v>
       </c>
-      <c r="BE90" t="s">
+      <c r="BF90" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="91" spans="1:57" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:58" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>489</v>
       </c>
@@ -9042,17 +9318,20 @@
       <c r="AF91" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="AJ91" s="6" t="s">
+      <c r="AJ91" t="s">
+        <v>618</v>
+      </c>
+      <c r="AK91" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="BD91" s="6" t="s">
+      <c r="BE91" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="BE91" s="6" t="s">
+      <c r="BF91" s="6" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>512</v>
       </c>
@@ -9107,14 +9386,17 @@
       <c r="AF92" t="s">
         <v>499</v>
       </c>
-      <c r="BD92" t="s">
+      <c r="AJ92" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE92" t="s">
         <v>597</v>
       </c>
-      <c r="BE92" t="s">
+      <c r="BF92" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="93" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>513</v>
       </c>
@@ -9169,14 +9451,17 @@
       <c r="AF93" t="s">
         <v>499</v>
       </c>
-      <c r="BD93" t="s">
+      <c r="AJ93" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE93" t="s">
         <v>600</v>
       </c>
-      <c r="BE93" t="s">
+      <c r="BF93" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="94" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>515</v>
       </c>
@@ -9231,14 +9516,17 @@
       <c r="AF94" t="s">
         <v>521</v>
       </c>
-      <c r="BD94" t="s">
+      <c r="AJ94" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE94" t="s">
         <v>601</v>
       </c>
-      <c r="BE94" t="s">
+      <c r="BF94" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="95" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>524</v>
       </c>
@@ -9293,8 +9581,11 @@
       <c r="AF95" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="96" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ95" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>531</v>
       </c>
@@ -9349,14 +9640,17 @@
       <c r="AF96" t="s">
         <v>499</v>
       </c>
-      <c r="BD96" t="s">
+      <c r="AJ96" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE96" t="s">
         <v>595</v>
       </c>
-      <c r="BE96" t="s">
+      <c r="BF96" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="97" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>533</v>
       </c>
@@ -9408,14 +9702,17 @@
       <c r="AF97" t="s">
         <v>539</v>
       </c>
-      <c r="BD97" t="s">
+      <c r="AJ97" t="s">
+        <v>618</v>
+      </c>
+      <c r="BE97" t="s">
         <v>595</v>
       </c>
-      <c r="BE97" t="s">
+      <c r="BF97" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="98" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>540</v>
       </c>
@@ -9473,8 +9770,11 @@
       <c r="AI98" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="99" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ98" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -9556,8 +9856,11 @@
       <c r="AI99" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="100" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ99" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -9648,8 +9951,11 @@
       <c r="AI100" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="101" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ100" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -9740,8 +10046,11 @@
       <c r="AI101" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="102" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ101" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>562</v>
       </c>
@@ -9802,8 +10111,11 @@
       <c r="AI102" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="103" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ102" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -9861,14 +10173,16 @@
       <c r="AI103" t="s">
         <v>603</v>
       </c>
+      <c r="AJ103" t="s">
+        <v>618</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="AH1:BE14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF103">
     <sortCondition ref="P2:P103"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mapas de ocorrência de invertebrados com pontos e mapas de espécies ameaçadas
</commit_message>
<xml_diff>
--- a/invertebrados/ocorrencias/Validado_Bivalvia_consolidado_05abr23.xlsx
+++ b/invertebrados/ocorrencias/Validado_Bivalvia_consolidado_05abr23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Taise\mapasAraguaia\invertebrados\ocorrencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE428431-4525-4823-819E-F8298B7A6794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D6C08F-34D8-49A2-857A-E71096386847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1836,9 +1836,6 @@
     <t>MMA, IN 05/04</t>
   </si>
   <si>
-    <t>BIODIVERSITAS,2002</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -1918,13 +1915,16 @@
   </si>
   <si>
     <t>nativo</t>
+  </si>
+  <si>
+    <t>categoria_iucn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1951,6 +1951,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2006,7 +2014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2014,6 +2022,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2328,12 +2337,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF103"/>
+  <dimension ref="A1:BI103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AX1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AE1" sqref="AE1"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="BI7" sqref="BI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,7 +2360,7 @@
     <col min="58" max="58" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2449,13 +2458,13 @@
         <v>31</v>
       </c>
       <c r="AH1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AI1" t="s">
         <v>569</v>
       </c>
       <c r="AJ1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="AK1" t="s">
         <v>570</v>
@@ -2521,10 +2530,10 @@
         <v>590</v>
       </c>
       <c r="BF1" s="4" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2598,7 +2607,7 @@
         <v>150</v>
       </c>
       <c r="AH2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ2" t="s">
         <v>588</v>
@@ -2610,7 +2619,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>304</v>
       </c>
@@ -2696,7 +2705,7 @@
         <v>296</v>
       </c>
       <c r="AH3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ3" t="s">
         <v>588</v>
@@ -2708,7 +2717,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>333</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>332</v>
       </c>
       <c r="AH4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ4" t="s">
         <v>588</v>
@@ -2806,7 +2815,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>370</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>375</v>
       </c>
       <c r="AH5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ5" t="s">
         <v>588</v>
@@ -2880,7 +2889,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>376</v>
       </c>
@@ -2942,7 +2951,7 @@
         <v>383</v>
       </c>
       <c r="AH6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ6" t="s">
         <v>588</v>
@@ -2954,7 +2963,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>384</v>
       </c>
@@ -3016,7 +3025,7 @@
         <v>389</v>
       </c>
       <c r="AH7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ7" t="s">
         <v>588</v>
@@ -3027,8 +3036,9 @@
       <c r="BC7" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="BI7" s="7"/>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>414</v>
       </c>
@@ -3081,7 +3091,7 @@
         <v>419</v>
       </c>
       <c r="AH8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ8" t="s">
         <v>588</v>
@@ -3093,7 +3103,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>435</v>
       </c>
@@ -3146,7 +3156,7 @@
         <v>439</v>
       </c>
       <c r="AH9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ9" t="s">
         <v>588</v>
@@ -3158,7 +3168,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>468</v>
       </c>
@@ -3220,7 +3230,7 @@
         <v>472</v>
       </c>
       <c r="AH10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ10" t="s">
         <v>588</v>
@@ -3232,7 +3242,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>473</v>
       </c>
@@ -3294,7 +3304,7 @@
         <v>477</v>
       </c>
       <c r="AH11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ11" t="s">
         <v>588</v>
@@ -3306,7 +3316,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>478</v>
       </c>
@@ -3368,7 +3378,7 @@
         <v>481</v>
       </c>
       <c r="AH12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ12" t="s">
         <v>588</v>
@@ -3380,7 +3390,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>482</v>
       </c>
@@ -3442,7 +3452,7 @@
         <v>485</v>
       </c>
       <c r="AH13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ13" t="s">
         <v>588</v>
@@ -3454,7 +3464,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>486</v>
       </c>
@@ -3516,7 +3526,7 @@
         <v>488</v>
       </c>
       <c r="AH14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AJ14" t="s">
         <v>588</v>
@@ -3528,7 +3538,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -3614,10 +3624,10 @@
         <v>51</v>
       </c>
       <c r="AJ15" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -3703,7 +3713,7 @@
         <v>51</v>
       </c>
       <c r="AJ16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.25">
@@ -3792,10 +3802,10 @@
         <v>51</v>
       </c>
       <c r="AJ17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
@@ -3881,10 +3891,10 @@
         <v>125</v>
       </c>
       <c r="AJ18" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK18" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.25">
@@ -3970,10 +3980,10 @@
         <v>167</v>
       </c>
       <c r="AJ19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.25">
@@ -4059,10 +4069,10 @@
         <v>175</v>
       </c>
       <c r="AJ20" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK20" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.25">
@@ -4148,10 +4158,10 @@
         <v>182</v>
       </c>
       <c r="AJ21" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK21" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.25">
@@ -4237,10 +4247,10 @@
         <v>189</v>
       </c>
       <c r="AJ22" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="23" spans="1:58" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4326,16 +4336,16 @@
         <v>202</v>
       </c>
       <c r="AJ23" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK23" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="BE23" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="BE23" s="5" t="s">
-        <v>609</v>
-      </c>
       <c r="BF23" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="24" spans="1:58" x14ac:dyDescent="0.25">
@@ -4424,7 +4434,7 @@
         <v>211</v>
       </c>
       <c r="AJ24" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.25">
@@ -4513,10 +4523,10 @@
         <v>231</v>
       </c>
       <c r="AJ25" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.25">
@@ -4605,7 +4615,7 @@
         <v>239</v>
       </c>
       <c r="AJ26" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.25">
@@ -4694,7 +4704,7 @@
         <v>263</v>
       </c>
       <c r="AJ27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.25">
@@ -4783,7 +4793,7 @@
         <v>274</v>
       </c>
       <c r="AJ28" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.25">
@@ -4872,7 +4882,7 @@
         <v>313</v>
       </c>
       <c r="AJ29" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.25">
@@ -4961,7 +4971,7 @@
         <v>284</v>
       </c>
       <c r="AJ30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.25">
@@ -5050,7 +5060,7 @@
         <v>290</v>
       </c>
       <c r="AJ31" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="32" spans="1:58" x14ac:dyDescent="0.25">
@@ -5139,7 +5149,7 @@
         <v>274</v>
       </c>
       <c r="AJ32" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
@@ -5228,7 +5238,7 @@
         <v>332</v>
       </c>
       <c r="AJ33" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
@@ -5311,7 +5321,7 @@
         <v>341</v>
       </c>
       <c r="AJ34" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
@@ -5397,7 +5407,7 @@
         <v>348</v>
       </c>
       <c r="AJ35" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
@@ -5483,7 +5493,7 @@
         <v>348</v>
       </c>
       <c r="AJ36" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
@@ -5569,10 +5579,10 @@
         <v>348</v>
       </c>
       <c r="AJ37" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK37" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
@@ -5658,7 +5668,7 @@
         <v>348</v>
       </c>
       <c r="AJ38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
@@ -5720,7 +5730,7 @@
         <v>395</v>
       </c>
       <c r="AJ39" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
@@ -5782,7 +5792,7 @@
         <v>395</v>
       </c>
       <c r="AJ40" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
@@ -5838,10 +5848,10 @@
         <v>408</v>
       </c>
       <c r="AJ41" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK41" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
@@ -5897,7 +5907,7 @@
         <v>413</v>
       </c>
       <c r="AJ42" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
@@ -5953,7 +5963,7 @@
         <v>424</v>
       </c>
       <c r="AJ43" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
@@ -6009,7 +6019,7 @@
         <v>429</v>
       </c>
       <c r="AJ44" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
@@ -6065,7 +6075,7 @@
         <v>434</v>
       </c>
       <c r="AJ45" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
@@ -6121,7 +6131,7 @@
         <v>419</v>
       </c>
       <c r="AJ46" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
@@ -6177,7 +6187,7 @@
         <v>448</v>
       </c>
       <c r="AJ47" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
@@ -6233,7 +6243,7 @@
         <v>455</v>
       </c>
       <c r="AJ48" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
@@ -6289,7 +6299,7 @@
         <v>460</v>
       </c>
       <c r="AJ49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
@@ -6345,7 +6355,7 @@
         <v>419</v>
       </c>
       <c r="AJ50" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
@@ -6404,7 +6414,7 @@
         <v>499</v>
       </c>
       <c r="AJ51" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
@@ -6463,7 +6473,7 @@
         <v>505</v>
       </c>
       <c r="AJ52" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
@@ -6522,7 +6532,7 @@
         <v>505</v>
       </c>
       <c r="AJ53" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
@@ -6581,7 +6591,7 @@
         <v>499</v>
       </c>
       <c r="AJ54" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
@@ -6640,7 +6650,7 @@
         <v>505</v>
       </c>
       <c r="AJ55" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
@@ -6699,7 +6709,7 @@
         <v>505</v>
       </c>
       <c r="AJ56" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
@@ -6758,7 +6768,7 @@
         <v>499</v>
       </c>
       <c r="AJ57" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
@@ -6817,7 +6827,7 @@
         <v>521</v>
       </c>
       <c r="AJ58" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
@@ -6876,7 +6886,7 @@
         <v>521</v>
       </c>
       <c r="AJ59" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
@@ -6932,10 +6942,10 @@
         <v>539</v>
       </c>
       <c r="AJ60" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK60" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
@@ -6991,7 +7001,7 @@
         <v>539</v>
       </c>
       <c r="AJ61" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
@@ -7047,7 +7057,7 @@
         <v>539</v>
       </c>
       <c r="AJ62" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
@@ -7103,7 +7113,7 @@
         <v>539</v>
       </c>
       <c r="AJ63" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
@@ -7159,7 +7169,7 @@
         <v>51</v>
       </c>
       <c r="AJ64" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="65" spans="1:58" x14ac:dyDescent="0.25">
@@ -7215,7 +7225,7 @@
         <v>51</v>
       </c>
       <c r="AJ65" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK65" t="s">
         <v>68</v>
@@ -7274,7 +7284,7 @@
         <v>51</v>
       </c>
       <c r="AJ66" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK66" t="s">
         <v>273</v>
@@ -7354,13 +7364,13 @@
         <v>136</v>
       </c>
       <c r="AH67" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI67" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="AJ67" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="68" spans="1:58" x14ac:dyDescent="0.25">
@@ -7416,13 +7426,13 @@
         <v>51</v>
       </c>
       <c r="AH68" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI68" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AJ68" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="69" spans="1:58" x14ac:dyDescent="0.25">
@@ -7478,16 +7488,16 @@
         <v>51</v>
       </c>
       <c r="AH69" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AJ69" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK69" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="70" spans="1:58" x14ac:dyDescent="0.25">
@@ -7534,16 +7544,16 @@
         <v>51</v>
       </c>
       <c r="AH70" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AJ70" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK70" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="71" spans="1:58" x14ac:dyDescent="0.25">
@@ -7623,13 +7633,13 @@
         <v>51</v>
       </c>
       <c r="AJ71" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE71" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF71" t="s">
         <v>595</v>
-      </c>
-      <c r="BF71" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="72" spans="1:58" x14ac:dyDescent="0.25">
@@ -7718,13 +7728,13 @@
         <v>51</v>
       </c>
       <c r="AH72" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI72" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AJ72" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="73" spans="1:58" x14ac:dyDescent="0.25">
@@ -7807,13 +7817,13 @@
         <v>158</v>
       </c>
       <c r="AJ73" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE73" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF73" t="s">
         <v>595</v>
-      </c>
-      <c r="BF73" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="74" spans="1:58" x14ac:dyDescent="0.25">
@@ -7902,13 +7912,13 @@
         <v>219</v>
       </c>
       <c r="AJ74" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE74" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF74" t="s">
         <v>595</v>
-      </c>
-      <c r="BF74" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="75" spans="1:58" x14ac:dyDescent="0.25">
@@ -7997,13 +8007,13 @@
         <v>225</v>
       </c>
       <c r="AJ75" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE75" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF75" t="s">
         <v>595</v>
-      </c>
-      <c r="BF75" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="76" spans="1:58" x14ac:dyDescent="0.25">
@@ -8092,13 +8102,13 @@
         <v>239</v>
       </c>
       <c r="AJ76" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE76" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF76" t="s">
         <v>595</v>
-      </c>
-      <c r="BF76" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="77" spans="1:58" x14ac:dyDescent="0.25">
@@ -8187,10 +8197,10 @@
         <v>251</v>
       </c>
       <c r="AJ77" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK77" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="78" spans="1:58" x14ac:dyDescent="0.25">
@@ -8279,13 +8289,13 @@
         <v>284</v>
       </c>
       <c r="AJ78" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE78" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="BF78" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="79" spans="1:58" x14ac:dyDescent="0.25">
@@ -8374,13 +8384,13 @@
         <v>290</v>
       </c>
       <c r="AJ79" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE79" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="BF79" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="80" spans="1:58" x14ac:dyDescent="0.25">
@@ -8469,13 +8479,13 @@
         <v>296</v>
       </c>
       <c r="AJ80" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE80" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="BF80" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="81" spans="1:58" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -8564,16 +8574,16 @@
         <v>284</v>
       </c>
       <c r="AJ81" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK81" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="BE81" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="BE81" s="6" t="s">
+      <c r="BF81" s="6" t="s">
         <v>605</v>
-      </c>
-      <c r="BF81" s="6" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="82" spans="1:58" x14ac:dyDescent="0.25">
@@ -8662,13 +8672,13 @@
         <v>326</v>
       </c>
       <c r="AJ82" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE82" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF82" t="s">
         <v>595</v>
-      </c>
-      <c r="BF82" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="83" spans="1:58" x14ac:dyDescent="0.25">
@@ -8754,13 +8764,13 @@
         <v>348</v>
       </c>
       <c r="AJ83" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE83" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF83" t="s">
         <v>595</v>
-      </c>
-      <c r="BF83" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="84" spans="1:58" x14ac:dyDescent="0.25">
@@ -8846,13 +8856,13 @@
         <v>348</v>
       </c>
       <c r="AJ84" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE84" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF84" t="s">
         <v>595</v>
-      </c>
-      <c r="BF84" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="85" spans="1:58" x14ac:dyDescent="0.25">
@@ -8938,7 +8948,7 @@
         <v>348</v>
       </c>
       <c r="AJ85" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="86" spans="1:58" x14ac:dyDescent="0.25">
@@ -9000,13 +9010,13 @@
         <v>395</v>
       </c>
       <c r="AJ86" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE86" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF86" t="s">
         <v>595</v>
-      </c>
-      <c r="BF86" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="87" spans="1:58" x14ac:dyDescent="0.25">
@@ -9068,7 +9078,7 @@
         <v>395</v>
       </c>
       <c r="AJ87" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="88" spans="1:58" x14ac:dyDescent="0.25">
@@ -9124,13 +9134,13 @@
         <v>439</v>
       </c>
       <c r="AJ88" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE88" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF88" t="s">
         <v>595</v>
-      </c>
-      <c r="BF88" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="89" spans="1:58" x14ac:dyDescent="0.25">
@@ -9186,13 +9196,13 @@
         <v>408</v>
       </c>
       <c r="AJ89" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE89" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF89" t="s">
         <v>595</v>
-      </c>
-      <c r="BF89" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="90" spans="1:58" x14ac:dyDescent="0.25">
@@ -9248,13 +9258,13 @@
         <v>467</v>
       </c>
       <c r="AJ90" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE90" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="BF90" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="91" spans="1:58" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -9319,16 +9329,16 @@
         <v>284</v>
       </c>
       <c r="AJ91" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AK91" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="BE91" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="BE91" s="6" t="s">
+      <c r="BF91" s="6" t="s">
         <v>605</v>
-      </c>
-      <c r="BF91" s="6" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="92" spans="1:58" x14ac:dyDescent="0.25">
@@ -9387,13 +9397,13 @@
         <v>499</v>
       </c>
       <c r="AJ92" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE92" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="BF92" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="93" spans="1:58" x14ac:dyDescent="0.25">
@@ -9452,13 +9462,13 @@
         <v>499</v>
       </c>
       <c r="AJ93" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE93" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="BF93" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="94" spans="1:58" x14ac:dyDescent="0.25">
@@ -9517,13 +9527,13 @@
         <v>521</v>
       </c>
       <c r="AJ94" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE94" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="BF94" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="95" spans="1:58" x14ac:dyDescent="0.25">
@@ -9582,7 +9592,7 @@
         <v>521</v>
       </c>
       <c r="AJ95" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="96" spans="1:58" x14ac:dyDescent="0.25">
@@ -9641,13 +9651,13 @@
         <v>499</v>
       </c>
       <c r="AJ96" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE96" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF96" t="s">
         <v>595</v>
-      </c>
-      <c r="BF96" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="97" spans="1:58" x14ac:dyDescent="0.25">
@@ -9703,13 +9713,13 @@
         <v>539</v>
       </c>
       <c r="AJ97" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BE97" t="s">
+        <v>594</v>
+      </c>
+      <c r="BF97" t="s">
         <v>595</v>
-      </c>
-      <c r="BF97" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="98" spans="1:58" x14ac:dyDescent="0.25">
@@ -9765,13 +9775,13 @@
         <v>539</v>
       </c>
       <c r="AH98" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI98" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AJ98" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="99" spans="1:58" x14ac:dyDescent="0.25">
@@ -9851,13 +9861,13 @@
         <v>96</v>
       </c>
       <c r="AH99" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI99" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AJ99" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="100" spans="1:58" x14ac:dyDescent="0.25">
@@ -9946,13 +9956,13 @@
         <v>96</v>
       </c>
       <c r="AH100" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI100" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AJ100" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="101" spans="1:58" x14ac:dyDescent="0.25">
@@ -10041,13 +10051,13 @@
         <v>96</v>
       </c>
       <c r="AH101" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI101" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AJ101" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="102" spans="1:58" x14ac:dyDescent="0.25">
@@ -10106,13 +10116,13 @@
         <v>96</v>
       </c>
       <c r="AH102" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI102" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AJ102" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="103" spans="1:58" x14ac:dyDescent="0.25">
@@ -10168,13 +10178,13 @@
         <v>51</v>
       </c>
       <c r="AH103" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AI103" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AJ103" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>